<commit_message>
ShadingPaints: Enlace entre la Vista de Pinturas y Datos de Pinturas
</commit_message>
<xml_diff>
--- a/ShadingPaints/spreadsheet/ShadingPaints.xlsx
+++ b/ShadingPaints/spreadsheet/ShadingPaints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58AC7CA9-16F4-4A7E-A1B7-37C7D0E2AE59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{172EAFA0-2CB6-4645-BB1B-C8E6D904B032}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3930" yWindow="-120" windowWidth="14400" windowHeight="7335" xr2:uid="{EFD61272-1A70-4617-AA0F-42EE7F191ECA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{EFD61272-1A70-4617-AA0F-42EE7F191ECA}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -604,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8573EC8-8B5F-4A74-B742-CE5C0A2EF676}">
   <dimension ref="A3:Q73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="C33" sqref="A33:XFD33"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="X67" sqref="X67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,46 +683,46 @@
         <v>0</v>
       </c>
       <c r="C5" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="D5" s="13">
         <v>950</v>
       </c>
       <c r="E5" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="F5" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="G5" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="H5" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I5" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="J5" s="13">
         <v>950</v>
       </c>
       <c r="K5" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="L5" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="M5" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="N5" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="P5" s="2">
         <v>2</v>
       </c>
       <c r="Q5" s="1">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -736,40 +736,40 @@
         <v>500</v>
       </c>
       <c r="E6" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="F6" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="G6" s="13">
         <v>950</v>
       </c>
       <c r="H6" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I6" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="J6" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="K6" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="L6" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="M6" s="13">
         <v>750</v>
       </c>
       <c r="N6" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="P6" s="2">
         <v>3</v>
       </c>
       <c r="Q6" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -777,10 +777,10 @@
         <v>2</v>
       </c>
       <c r="C7" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="D7" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="E7" s="13">
         <v>850</v>
@@ -789,16 +789,16 @@
         <v>500</v>
       </c>
       <c r="G7" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="H7" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I7" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="J7" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="K7" s="13">
         <v>500</v>
@@ -807,16 +807,16 @@
         <v>850</v>
       </c>
       <c r="M7" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="N7" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="P7" s="2">
+        <v>3</v>
+      </c>
+      <c r="Q7" s="1">
         <v>4</v>
-      </c>
-      <c r="Q7" s="1">
-        <v>5</v>
       </c>
     </row>
     <row r="8" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -824,37 +824,37 @@
         <v>3</v>
       </c>
       <c r="C8" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="D8" s="13">
         <v>750</v>
       </c>
       <c r="E8" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="F8" s="13">
         <v>500</v>
       </c>
       <c r="G8" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="H8" s="13">
         <v>500</v>
       </c>
       <c r="I8" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="J8" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="K8" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="L8" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="M8" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="N8" s="13">
         <v>950</v>
@@ -863,7 +863,7 @@
         <v>5</v>
       </c>
       <c r="Q8" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -871,43 +871,43 @@
         <v>14</v>
       </c>
       <c r="C9" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="D9" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="E9" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="F9" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="G9" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="H9" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I9" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="J9" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="K9" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="L9" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="M9" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="N9" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="P9" s="2">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="Q9" s="1">
         <v>3</v>
@@ -918,10 +918,10 @@
         <v>4</v>
       </c>
       <c r="C10" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="D10" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="E10" s="13">
         <v>850</v>
@@ -930,13 +930,13 @@
         <v>500</v>
       </c>
       <c r="G10" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="H10" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I10" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="J10" s="13">
         <v>500</v>
@@ -948,7 +948,7 @@
         <v>950</v>
       </c>
       <c r="M10" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="N10" s="13">
         <v>1050</v>
@@ -957,7 +957,7 @@
         <v>1</v>
       </c>
       <c r="Q10" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -965,46 +965,46 @@
         <v>15</v>
       </c>
       <c r="C11" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="D11" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="E11" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="F11" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="G11" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="H11" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I11" s="13">
         <v>850</v>
       </c>
       <c r="J11" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="K11" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="L11" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="M11" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="N11" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="P11" s="2">
         <v>2</v>
       </c>
       <c r="Q11" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1012,16 +1012,16 @@
         <v>16</v>
       </c>
       <c r="C12" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="D12" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="E12" s="13">
         <v>500</v>
       </c>
       <c r="F12" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="G12" s="13">
         <v>750</v>
@@ -1030,28 +1030,28 @@
         <v>750</v>
       </c>
       <c r="I12" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="J12" s="13">
         <v>1050</v>
       </c>
       <c r="K12" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="L12" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="M12" s="13">
         <v>850</v>
       </c>
       <c r="N12" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="P12" s="2">
         <v>1</v>
       </c>
       <c r="Q12" s="1">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1059,46 +1059,46 @@
         <v>17</v>
       </c>
       <c r="C13" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="D13" s="13">
         <v>750</v>
       </c>
       <c r="E13" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="F13" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="G13" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="H13" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I13" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="J13" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="K13" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="L13" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="M13" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="N13" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="P13" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q13" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1109,13 +1109,13 @@
         <v>500</v>
       </c>
       <c r="D14" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="E14" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="F14" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="G14" s="13">
         <v>950</v>
@@ -1130,22 +1130,22 @@
         <v>750</v>
       </c>
       <c r="K14" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="L14" s="13">
         <v>1050</v>
       </c>
       <c r="M14" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="N14" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="P14" s="2">
         <v>1</v>
       </c>
       <c r="Q14" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1153,46 +1153,46 @@
         <v>22</v>
       </c>
       <c r="C15" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="D15" s="13">
         <v>950</v>
       </c>
       <c r="E15" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="F15" s="13">
         <v>750</v>
       </c>
       <c r="G15" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="H15" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I15" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="J15" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="K15" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="L15" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="M15" s="13">
         <v>500</v>
       </c>
       <c r="N15" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="P15" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Q15" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1200,46 +1200,46 @@
         <v>23</v>
       </c>
       <c r="C16" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="D16" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="E16" s="13">
         <v>950</v>
       </c>
       <c r="F16" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="G16" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="H16" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I16" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="J16" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="K16" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="L16" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="M16" s="13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="N16" s="13">
         <v>1050</v>
       </c>
       <c r="P16" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q16" s="1">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1248,40 +1248,40 @@
         <v>19</v>
       </c>
       <c r="C18" s="1">
-        <v>80000</v>
+        <v>200000</v>
       </c>
       <c r="D18" s="1">
-        <v>80000</v>
+        <v>200000</v>
       </c>
       <c r="E18" s="1">
-        <v>80000</v>
+        <v>200000</v>
       </c>
       <c r="F18" s="1">
-        <v>80000</v>
+        <v>200000</v>
       </c>
       <c r="G18" s="1">
-        <v>80000</v>
+        <v>200000</v>
       </c>
       <c r="H18" s="1">
-        <v>80000</v>
+        <v>200000</v>
       </c>
       <c r="I18" s="1">
-        <v>80000</v>
+        <v>200000</v>
       </c>
       <c r="J18" s="1">
-        <v>80000</v>
+        <v>200000</v>
       </c>
       <c r="K18" s="1">
-        <v>80000</v>
+        <v>200000</v>
       </c>
       <c r="L18" s="1">
-        <v>80000</v>
+        <v>200000</v>
       </c>
       <c r="M18" s="1">
-        <v>80000</v>
+        <v>200000</v>
       </c>
       <c r="N18" s="1">
-        <v>80000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
@@ -1978,40 +1978,40 @@
         <v>0</v>
       </c>
       <c r="C47" s="1">
-        <v>1150</v>
+        <v>650</v>
       </c>
       <c r="D47" s="1">
         <v>950</v>
       </c>
       <c r="E47" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="F47" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="G47" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="H47" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I47" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="J47" s="1">
         <v>950</v>
       </c>
       <c r="K47" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="L47" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="M47" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="N47" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2022,37 +2022,37 @@
         <v>900</v>
       </c>
       <c r="D48" s="1">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="E48" s="1">
         <v>0</v>
       </c>
       <c r="F48" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="G48" s="1">
         <v>950</v>
       </c>
       <c r="H48" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I48" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="J48" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="K48" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="L48" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="M48" s="1">
         <v>750</v>
       </c>
       <c r="N48" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="49" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2060,7 +2060,7 @@
         <v>2</v>
       </c>
       <c r="C49" s="1">
-        <v>2150</v>
+        <v>1150</v>
       </c>
       <c r="D49" s="1">
         <v>0</v>
@@ -2072,16 +2072,16 @@
         <v>500</v>
       </c>
       <c r="G49" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="H49" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I49" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="J49" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="K49" s="1">
         <v>500</v>
@@ -2090,10 +2090,10 @@
         <v>850</v>
       </c>
       <c r="M49" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="N49" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="50" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2101,37 +2101,37 @@
         <v>3</v>
       </c>
       <c r="C50" s="1">
-        <v>1150</v>
+        <v>650</v>
       </c>
       <c r="D50" s="1">
         <v>750</v>
       </c>
       <c r="E50" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="F50" s="1">
         <v>500</v>
       </c>
       <c r="G50" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="H50" s="1">
         <v>500</v>
       </c>
       <c r="I50" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="J50" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="K50" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="L50" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="M50" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="N50" s="1">
         <v>950</v>
@@ -2142,13 +2142,13 @@
         <v>14</v>
       </c>
       <c r="C51" s="1">
-        <v>1150</v>
+        <v>650</v>
       </c>
       <c r="D51" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="E51" s="1">
-        <v>4000</v>
+        <v>2000</v>
       </c>
       <c r="F51" s="1">
         <v>0</v>
@@ -2160,22 +2160,22 @@
         <v>0</v>
       </c>
       <c r="I51" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="J51" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="K51" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="L51" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="M51" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="N51" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="52" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2183,10 +2183,10 @@
         <v>4</v>
       </c>
       <c r="C52" s="1">
-        <v>1150</v>
+        <v>650</v>
       </c>
       <c r="D52" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="E52" s="1">
         <v>850</v>
@@ -2195,13 +2195,13 @@
         <v>500</v>
       </c>
       <c r="G52" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="H52" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I52" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="J52" s="1">
         <v>500</v>
@@ -2213,7 +2213,7 @@
         <v>950</v>
       </c>
       <c r="M52" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="N52" s="1">
         <v>1050</v>
@@ -2224,40 +2224,40 @@
         <v>15</v>
       </c>
       <c r="C53" s="1">
-        <v>1150</v>
+        <v>650</v>
       </c>
       <c r="D53" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="E53" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="F53" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="G53" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="H53" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I53" s="1">
         <v>850</v>
       </c>
       <c r="J53" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="K53" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="L53" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="M53" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="N53" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="54" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2265,16 +2265,16 @@
         <v>16</v>
       </c>
       <c r="C54" s="1">
-        <v>1150</v>
+        <v>650</v>
       </c>
       <c r="D54" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="E54" s="1">
         <v>500</v>
       </c>
       <c r="F54" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="G54" s="1">
         <v>1500</v>
@@ -2283,22 +2283,22 @@
         <v>0</v>
       </c>
       <c r="I54" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="J54" s="1">
         <v>1050</v>
       </c>
       <c r="K54" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="L54" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="M54" s="1">
         <v>850</v>
       </c>
       <c r="N54" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="55" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2306,40 +2306,40 @@
         <v>17</v>
       </c>
       <c r="C55" s="1">
-        <v>1150</v>
+        <v>650</v>
       </c>
       <c r="D55" s="1">
         <v>750</v>
       </c>
       <c r="E55" s="1">
+        <v>500</v>
+      </c>
+      <c r="F55" s="1">
+        <v>500</v>
+      </c>
+      <c r="G55" s="1">
         <v>1000</v>
-      </c>
-      <c r="F55" s="1">
-        <v>1000</v>
-      </c>
-      <c r="G55" s="1">
-        <v>2000</v>
       </c>
       <c r="H55" s="1">
         <v>0</v>
       </c>
       <c r="I55" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="J55" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="K55" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="L55" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="M55" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="N55" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="56" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2350,13 +2350,13 @@
         <v>650</v>
       </c>
       <c r="D56" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="E56" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="F56" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="G56" s="1">
         <v>1800</v>
@@ -2371,16 +2371,16 @@
         <v>750</v>
       </c>
       <c r="K56" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="L56" s="1">
         <v>1050</v>
       </c>
       <c r="M56" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="N56" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="57" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2388,10 +2388,10 @@
         <v>22</v>
       </c>
       <c r="C57" s="1">
-        <v>1150</v>
+        <v>650</v>
       </c>
       <c r="D57" s="1">
-        <v>1950</v>
+        <v>1450</v>
       </c>
       <c r="E57" s="1">
         <v>0</v>
@@ -2400,28 +2400,28 @@
         <v>750</v>
       </c>
       <c r="G57" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="H57" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I57" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="J57" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="K57" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="L57" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="M57" s="1">
         <v>500</v>
       </c>
       <c r="N57" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="58" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2429,37 +2429,37 @@
         <v>23</v>
       </c>
       <c r="C58" s="1">
-        <v>1150</v>
+        <v>650</v>
       </c>
       <c r="D58" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="E58" s="1">
         <v>950</v>
       </c>
       <c r="F58" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="G58" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="H58" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I58" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="J58" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="K58" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="L58" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="M58" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="N58" s="1">
         <v>1050</v>
@@ -2572,7 +2572,7 @@
         <v>150</v>
       </c>
       <c r="D63" s="1">
-        <v>1150</v>
+        <v>650</v>
       </c>
       <c r="E63" s="1">
         <v>150</v>
@@ -2610,7 +2610,7 @@
         <v>2</v>
       </c>
       <c r="C64" s="1">
-        <v>1150</v>
+        <v>650</v>
       </c>
       <c r="D64" s="1">
         <v>150</v>
@@ -2698,13 +2698,13 @@
         <v>150</v>
       </c>
       <c r="E66" s="1">
-        <v>3150</v>
+        <v>1650</v>
       </c>
       <c r="F66" s="1">
-        <v>2150</v>
+        <v>1150</v>
       </c>
       <c r="G66" s="1">
-        <v>1150</v>
+        <v>650</v>
       </c>
       <c r="H66" s="1">
         <v>150</v>
@@ -2868,7 +2868,7 @@
         <v>150</v>
       </c>
       <c r="G70" s="1">
-        <v>1150</v>
+        <v>650</v>
       </c>
       <c r="H70" s="1">
         <v>150</v>
@@ -2941,7 +2941,7 @@
         <v>150</v>
       </c>
       <c r="D72" s="1">
-        <v>1150</v>
+        <v>650</v>
       </c>
       <c r="E72" s="1">
         <v>150</v>

</xml_diff>